<commit_message>
DMS POSM WITHDRAW: update export template
</commit_message>
<xml_diff>
--- a/DMS/Templates/POSMWITHDRAW_Export.xlsx
+++ b/DMS/Templates/POSMWITHDRAW_Export.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\BE\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0373D5-5AED-4C4B-AA6C-553937CAC986}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797898D0-7765-4380-81AF-864025434820}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,33 +84,9 @@
     <t>{{Data.Store.Address}}</t>
   </si>
   <si>
-    <t>{{Data.Total}}</t>
-  </si>
-  <si>
     <t>{{Data.Store.StoreStatus.Name}}</t>
   </si>
   <si>
-    <t>{{Data.Stores.ShowingOrderContents.ShowingItem.Code}}</t>
-  </si>
-  <si>
-    <t>{{Data.Stores.ShowingOrderContents.ShowingItem.Name}}</t>
-  </si>
-  <si>
-    <t>{{Data.Stores.ShowingOrderContents.ShowingItem.ShowingCategory.Name}}</t>
-  </si>
-  <si>
-    <t>{{Data.Stores.ShowingOrderContents.UnitOfMeasure.Name}}</t>
-  </si>
-  <si>
-    <t>{{Data.Stores.ShowingOrderContents.SalePrice}}</t>
-  </si>
-  <si>
-    <t>{{Data.Stores.ShowingOrderContents.Quantity}}</t>
-  </si>
-  <si>
-    <t>{{Data.Stores.ShowingOrderContents.Amount}}</t>
-  </si>
-  <si>
     <t>{{Data.Organization.Name}}</t>
   </si>
   <si>
@@ -123,10 +99,34 @@
     <t>Tổng giá trị thu hồi</t>
   </si>
   <si>
-    <t>{{Data.Date}}</t>
-  </si>
-  <si>
     <t>Ngày thu hồi</t>
+  </si>
+  <si>
+    <t>{{Data.eDate}}</t>
+  </si>
+  <si>
+    <t>{{Data.eTotal}}</t>
+  </si>
+  <si>
+    <t>{{Data.ShowingOrderContentWithDraws.eSalePrice}}</t>
+  </si>
+  <si>
+    <t>{{Data.ShowingOrderContentWithDraws.eQuantity}}</t>
+  </si>
+  <si>
+    <t>{{Data.ShowingOrderContentWithDraws.eAmount}}</t>
+  </si>
+  <si>
+    <t>{{Data.ShowingOrderContentWithDraws.ShowingItem.Code}}</t>
+  </si>
+  <si>
+    <t>{{Data.ShowingOrderContentWithDraws.ShowingItem.Name}}</t>
+  </si>
+  <si>
+    <t>{{Data.ShowingOrderContentWithDraws.ShowingItem.ShowingCategory.Name}}</t>
+  </si>
+  <si>
+    <t>{{Data.ShowingOrderContentWithDraws.UnitOfMeasure.Name}}</t>
   </si>
 </sst>
 </file>
@@ -184,7 +184,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -262,22 +262,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -300,9 +289,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -323,9 +309,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,276 +590,295 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X9"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:G9"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="3.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="3" customWidth="1"/>
-    <col min="4" max="5" width="8.7109375" style="3" customWidth="1"/>
-    <col min="6" max="7" width="11.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="3" customWidth="1"/>
-    <col min="10" max="11" width="14.7109375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.42578125" style="3" customWidth="1"/>
-    <col min="15" max="15" width="15.140625" style="3" customWidth="1"/>
-    <col min="16" max="17" width="28.28515625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="16.28515625" style="3" customWidth="1"/>
-    <col min="19" max="19" width="14" style="3" customWidth="1"/>
-    <col min="20" max="20" width="13.140625" style="3" customWidth="1"/>
-    <col min="21" max="21" width="14.140625" style="3" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="3"/>
+    <col min="3" max="4" width="14.28515625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="8.7109375" style="3" customWidth="1"/>
+    <col min="7" max="8" width="11.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="3" customWidth="1"/>
+    <col min="11" max="12" width="14.7109375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" style="3" customWidth="1"/>
+    <col min="15" max="16" width="10.42578125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="28.28515625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="16.28515625" style="3" customWidth="1"/>
+    <col min="21" max="21" width="14" style="3" customWidth="1"/>
+    <col min="22" max="22" width="13.140625" style="3" customWidth="1"/>
+    <col min="23" max="23" width="14.140625" style="3" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="5"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="5"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="5"/>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="5"/>
     </row>
-    <row r="4" spans="1:24" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:26" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+    </row>
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+    </row>
+    <row r="7" spans="1:26" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7" s="9"/>
+      <c r="M7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" s="9"/>
+      <c r="O7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+    </row>
+    <row r="9" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-    </row>
-    <row r="5" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-    </row>
-    <row r="7" spans="1:24" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="16" t="s">
+      <c r="R9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="S9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="T9" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="N7" s="10"/>
-      <c r="O7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
-    </row>
-    <row r="9" spans="1:24" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" s="8"/>
-      <c r="L9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="N9" s="8"/>
-      <c r="O9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="R9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="S9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="T9" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="U9" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="V9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="W9" s="6" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="A4:U4"/>
-    <mergeCell ref="A8:U8"/>
+  <mergeCells count="21">
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A4:W4"/>
+    <mergeCell ref="A8:W8"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="M7:N7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="A5:W5"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="C9:D9"/>
     <mergeCell ref="M9:N9"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="A5:U5"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
DMS: Fix POSM template
</commit_message>
<xml_diff>
--- a/DMS/Templates/POSMWITHDRAW_Export.xlsx
+++ b/DMS/Templates/POSMWITHDRAW_Export.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\BE\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797898D0-7765-4380-81AF-864025434820}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471ACA8A-16F6-4D4C-B989-5F0D4C14206E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>STT</t>
   </si>
@@ -127,13 +127,25 @@
   </si>
   <si>
     <t>{{Data.ShowingOrderContentWithDraws.UnitOfMeasure.Name}}</t>
+  </si>
+  <si>
+    <t>Người tạo</t>
+  </si>
+  <si>
+    <t>{{Data.AppUser.DisplayName}}</t>
+  </si>
+  <si>
+    <t>Tổng</t>
+  </si>
+  <si>
+    <t>{{Total}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +181,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -266,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -287,7 +305,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -295,6 +322,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -309,6 +339,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -590,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z9"/>
+  <dimension ref="A1:AB10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10:R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,278 +640,311 @@
     <col min="10" max="10" width="12.42578125" style="3" customWidth="1"/>
     <col min="11" max="12" width="14.7109375" style="3" customWidth="1"/>
     <col min="13" max="13" width="19.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" style="3" customWidth="1"/>
-    <col min="15" max="16" width="10.42578125" style="3" customWidth="1"/>
-    <col min="17" max="17" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="28.28515625" style="3" customWidth="1"/>
-    <col min="20" max="20" width="16.28515625" style="3" customWidth="1"/>
-    <col min="21" max="21" width="14" style="3" customWidth="1"/>
-    <col min="22" max="22" width="13.140625" style="3" customWidth="1"/>
-    <col min="23" max="23" width="14.140625" style="3" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="3"/>
+    <col min="14" max="15" width="19.140625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="4.85546875" style="3" customWidth="1"/>
+    <col min="17" max="18" width="10.42578125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="28.28515625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="16.28515625" style="3" customWidth="1"/>
+    <col min="23" max="23" width="14" style="3" customWidth="1"/>
+    <col min="24" max="24" width="13.140625" style="3" customWidth="1"/>
+    <col min="25" max="25" width="14.140625" style="3" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="5"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="5"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="5"/>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="5"/>
     </row>
-    <row r="4" spans="1:26" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:28" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
     </row>
-    <row r="7" spans="1:26" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:28" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="8" t="s">
+      <c r="D7" s="12"/>
+      <c r="E7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="8" t="s">
+      <c r="F7" s="12"/>
+      <c r="G7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="8" t="s">
+      <c r="H7" s="12"/>
+      <c r="I7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="9"/>
-      <c r="K7" s="8" t="s">
+      <c r="J7" s="12"/>
+      <c r="K7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="9"/>
-      <c r="M7" s="8" t="s">
+      <c r="L7" s="12"/>
+      <c r="M7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="N7" s="9"/>
-      <c r="O7" s="8" t="s">
+      <c r="N7" s="12"/>
+      <c r="O7" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="1" t="s">
+      <c r="R7" s="12"/>
+      <c r="S7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="V7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="W7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="X7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="Y7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="4"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="18"/>
       <c r="Z8" s="4"/>
+      <c r="AA8" s="4"/>
+      <c r="AB8" s="4"/>
     </row>
-    <row r="9" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7" t="s">
+      <c r="D9" s="13"/>
+      <c r="E9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7" t="s">
+      <c r="F9" s="13"/>
+      <c r="G9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7" t="s">
+      <c r="H9" s="13"/>
+      <c r="I9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7" t="s">
+      <c r="J9" s="13"/>
+      <c r="K9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7" t="s">
+      <c r="L9" s="13"/>
+      <c r="M9" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7" t="s">
+      <c r="N9" s="13"/>
+      <c r="O9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="6" t="s">
+      <c r="R9" s="10"/>
+      <c r="S9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="R9" s="6" t="s">
+      <c r="T9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="S9" s="6" t="s">
+      <c r="U9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="T9" s="6" t="s">
+      <c r="V9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="U9" s="6" t="s">
+      <c r="W9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="V9" s="6" t="s">
+      <c r="X9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="W9" s="6" t="s">
+      <c r="Y9" s="7" t="s">
         <v>29</v>
       </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="Q10" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="R10" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A4:W4"/>
-    <mergeCell ref="A8:W8"/>
+  <mergeCells count="25">
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A4:Y4"/>
+    <mergeCell ref="A8:Y8"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="G7:H7"/>
-    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:R7"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="A5:W5"/>
+    <mergeCell ref="A5:Y5"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K9:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>